<commit_message>
1) Implement database structure for templates. 2) Implement database structure for Test Case Types to allow classification (i.e. Module, Integration, etc. (GAMP 5))
</commit_message>
<xml_diff>
--- a/VM-Core/src/test/java/com/validation/manager/core/tool/requirement/importer/Header.xlsx
+++ b/VM-Core/src/test/java/com/validation/manager/core/tool/requirement/importer/Header.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="23952" windowHeight="10032"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>SRS-SW-001</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Description 20</t>
   </si>
   <si>
-    <t>SW</t>
-  </si>
-  <si>
     <t>Notes 1</t>
   </si>
   <si>
@@ -202,13 +199,16 @@
   </si>
   <si>
     <t>Header</t>
+  </si>
+  <si>
+    <t>MS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +245,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -323,6 +328,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -357,6 +363,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,25 +539,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -558,13 +565,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -572,13 +579,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -586,13 +593,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -600,13 +607,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -614,13 +621,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -628,13 +635,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -642,13 +649,13 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -656,13 +663,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -670,13 +677,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -684,13 +691,13 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -698,24 +705,27 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
       <c r="D13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -723,13 +733,13 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -737,13 +747,13 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -751,13 +761,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -765,13 +775,13 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -779,13 +789,13 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -793,13 +803,13 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -807,13 +817,13 @@
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -821,10 +831,10 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -833,24 +843,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Release version 0.3.5 (#83)
## New Features
- Export Trace Matrix
- Export Test Plan
- Export Attachments with Test Case Execution Export
- Have templates based on project type
- Project Templates
- Add about tab

## Bug fixes
- Error creating issue during execution
- Unable to create requirement
- Login in with multiple windows open cause runtime error
- Updating project doesn't work
</commit_message>
<xml_diff>
--- a/VM-Core/src/test/java/com/validation/manager/core/tool/requirement/importer/Header.xlsx
+++ b/VM-Core/src/test/java/com/validation/manager/core/tool/requirement/importer/Header.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="23955" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="23952" windowHeight="10032"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>SRS-SW-001</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Description 20</t>
   </si>
   <si>
-    <t>SW</t>
-  </si>
-  <si>
     <t>Notes 1</t>
   </si>
   <si>
@@ -202,13 +199,16 @@
   </si>
   <si>
     <t>Header</t>
+  </si>
+  <si>
+    <t>MS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +245,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -323,6 +328,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -357,6 +363,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,25 +539,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -558,13 +565,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -572,13 +579,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -586,13 +593,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -600,13 +607,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -614,13 +621,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -628,13 +635,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -642,13 +649,13 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -656,13 +663,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -670,13 +677,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -684,13 +691,13 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -698,24 +705,27 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
       <c r="D13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -723,13 +733,13 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -737,13 +747,13 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -751,13 +761,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -765,13 +775,13 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -779,13 +789,13 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -793,13 +803,13 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -807,13 +817,13 @@
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -821,10 +831,10 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -833,24 +843,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>